<commit_message>
Update excel input files; Add working directory
</commit_message>
<xml_diff>
--- a/data/usda irrigation water requirement.xlsx
+++ b/data/usda irrigation water requirement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoon644\OneDrive - PNNL\Documents\PyProjects\wm-abm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/jim_yoon_pnnl_gov/Documents/Documents/PyProjects/wm-abm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{2040F1DA-0E17-9B40-A4C2-C9CDA6B17712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{72E9F4FA-868F-4F72-8A8D-77F6F2B70A78}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{2040F1DA-0E17-9B40-A4C2-C9CDA6B17712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{367B8E9F-1CCD-45FD-8FF4-AFEE9487347C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{55C1A0D5-D700-FA4B-B000-64EB1C769A29}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{55C1A0D5-D700-FA4B-B000-64EB1C769A29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>